<commit_message>
added more manual tests and a protocol for some tests i did today
</commit_message>
<xml_diff>
--- a/documents/tests/Manuelle Systemtests.xlsx
+++ b/documents/tests/Manuelle Systemtests.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="68">
   <si>
     <t>Manuelle Systemtests Documentation</t>
   </si>
@@ -172,6 +172,69 @@
   </si>
   <si>
     <t>Sonderfall (SF)</t>
+  </si>
+  <si>
+    <t>Pagination in Kunden Tab</t>
+  </si>
+  <si>
+    <t>es existieren mehr als 20 Kunden im System (am besten &gt; 100 Kunden)</t>
+  </si>
+  <si>
+    <t>Pagination in Event / Performance Tab</t>
+  </si>
+  <si>
+    <t>Pagination in Transaktionen Tab</t>
+  </si>
+  <si>
+    <t>Pagination in der Kundenauswahl nach dem Saalplan</t>
+  </si>
+  <si>
+    <t>es existieren mehr als 20 Events im System</t>
+  </si>
+  <si>
+    <t>es existieren mehr als 20 Transaktionen im System</t>
+  </si>
+  <si>
+    <t>es existieren mehr als 20 Kunden im System</t>
+  </si>
+  <si>
+    <t>Kunden-Tab öffnen, dabei werden 20 Einträge geladen, dann nach unten scrollen</t>
+  </si>
+  <si>
+    <t>Transaktionen-Tab öffnen, dabei werden 20 Einträge geladen, dann nach unten scrollen</t>
+  </si>
+  <si>
+    <t>die nächsten 20 Einträge werden geladen usw.</t>
+  </si>
+  <si>
+    <t>Ein Event auswählen, Plätze / Sektoren im Saalplan auswählen und weiter zur Kundenauswahl - dort nach unten scrollen</t>
+  </si>
+  <si>
+    <t>Event-Tab öffnen, dabei werden 20 Einträge geladen, dann nach unten scrollen</t>
+  </si>
+  <si>
+    <t>Sprache ändern während des Betriebs</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>während der Verwendung des Programms im Menü (oben) auf Sprache und auf die andere Sprache wechseln</t>
+  </si>
+  <si>
+    <t>alles soll sofort auf die neue Sprache umgestellt sein und auch neue Fenster/Tabs sollen in der neuen Sprache geöffnet werden</t>
+  </si>
+  <si>
+    <t>Kundenauswahl nach Saalplan - Kunde wird angelegt und ist danach markiert und ausgewählt</t>
+  </si>
+  <si>
+    <t>es existiert zumindest ein Event mit einer Performance - diese auswählen und Tickets dazu auswählen, danach auf Weiter klicken zur Kundenauswahl</t>
+  </si>
+  <si>
+    <t>Klick auf Kunde hinzufügen, neuen Kunden einfügen - danach schließt sich Fenster wieder</t>
+  </si>
+  <si>
+    <t>neu angelegter Kunde ist ausgewählt und nach bei einer Suche nach dem Kunden auch markiert</t>
   </si>
 </sst>
 </file>
@@ -407,10 +470,10 @@
   <tableColumns count="6">
     <tableColumn id="1" name="Testfall #" dataDxfId="5"/>
     <tableColumn id="2" name="Testtyp" dataDxfId="4"/>
-    <tableColumn id="3" name="Kurzbeschreibung" dataDxfId="2"/>
-    <tableColumn id="4" name="Vorbedingungen" dataDxfId="1"/>
-    <tableColumn id="5" name="Eingaben" dataDxfId="0"/>
-    <tableColumn id="6" name="Erwartetes Ergebnis" dataDxfId="3"/>
+    <tableColumn id="3" name="Kurzbeschreibung" dataDxfId="3"/>
+    <tableColumn id="4" name="Vorbedingungen" dataDxfId="2"/>
+    <tableColumn id="5" name="Eingaben" dataDxfId="1"/>
+    <tableColumn id="6" name="Erwartetes Ergebnis" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -681,14 +744,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G400"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="15.7109375" style="1" customWidth="1"/>
-    <col min="3" max="6" width="30.7109375" style="8" customWidth="1"/>
+    <col min="3" max="5" width="30.7109375" style="8" customWidth="1"/>
+    <col min="6" max="6" width="35" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -940,23 +1004,125 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-    </row>
-    <row r="20" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
-    </row>
-    <row r="21" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
-    </row>
-    <row r="22" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
-    </row>
-    <row r="23" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
-    </row>
-    <row r="24" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
+    <row r="19" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="6">
+        <v>10</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="6">
+        <v>11</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="6">
+        <v>12</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A22" s="6">
+        <v>13</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="6">
+        <v>14</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A24" s="6">
+        <v>15</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="25" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>

</xml_diff>

<commit_message>
changed news limits (summary limit is now 1000 chars) and checks and added new tests and questions
</commit_message>
<xml_diff>
--- a/documents/tests/Manuelle Systemtests.xlsx
+++ b/documents/tests/Manuelle Systemtests.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\University\proj_ss17_sepm_inso_07\documents\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Martin\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2580" yWindow="2400" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14535" windowHeight="12270"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="90">
   <si>
     <t>Manuelle Systemtests Documentation</t>
   </si>
@@ -235,6 +235,72 @@
   </si>
   <si>
     <t>neu angelegter Kunde ist ausgewählt und nach bei einer Suche nach dem Kunden auch markiert</t>
+  </si>
+  <si>
+    <t>alle News anzeigen</t>
+  </si>
+  <si>
+    <t>alle ungelesenen News anzeigen</t>
+  </si>
+  <si>
+    <t>neuen News Beitrag ohne Bild erstellen</t>
+  </si>
+  <si>
+    <t>neuen News Beitrag mit Bild erstellen</t>
+  </si>
+  <si>
+    <t>neuen News Beitrag mit einem Bild &gt; 5 MB erstellen</t>
+  </si>
+  <si>
+    <t>es gibt bereits mehr als 20 News Einträge im System</t>
+  </si>
+  <si>
+    <t>einen News Eintrag öffnen - danach wieder schließen, danach unten auf "Gelesene Anzeigen?" klicken</t>
+  </si>
+  <si>
+    <t>der gerade gelesene Eintrag sollte auch zu sehen sein und beim nach unten scrollen sollten gepaged alle News geladen werden</t>
+  </si>
+  <si>
+    <t>einen News Eintrag öffnen und danach wieder schließen</t>
+  </si>
+  <si>
+    <t>der gerade gelesene Eintrag ist jetzt nicht mehr in der Liste, beim nach unten scrollen werden die nächsten ungelesenen News gepaged geladen</t>
+  </si>
+  <si>
+    <t>neuen unvollständigen News Beitrag erstellen</t>
+  </si>
+  <si>
+    <t>Klick auf "News hinzufügen" und alle Felder bis auf das Bild ausfüllen und mit News veröffentlichen bestätigen</t>
+  </si>
+  <si>
+    <t>das Fenster schließt sich und der Beitrag wird ganz oben angezeigt (als ungelesener Beitrag)</t>
+  </si>
+  <si>
+    <t>das Fenster schließt sich und der Beitrag wird ganz oben angezeigt (als ungelesener Beitrag) - wenn man diesen nun öffnet sieht man auch das Bild</t>
+  </si>
+  <si>
+    <t>Klick auf "News hinzufügen" und entweder Titel, Zusammenfassung oder Text nicht ausfüllen und mit News veröffentlichen bestätigen</t>
+  </si>
+  <si>
+    <t>neuen News Beitrag erstellen mit zu langen Texten</t>
+  </si>
+  <si>
+    <t>Klick auf "News hinzufügen" und entweder beim Titel mehr als 100 Zeichen, bei der Zusammenfassung mehr als 1.000 oder beim Text mehr als 10.000 Zeichen eintragen und mit News veröffentlichen bestätigen</t>
+  </si>
+  <si>
+    <t>Klick auf "News hinzufügen" und alle Felder inklusive einem Bild (kleiner als 5 MB) ausfüllen und mit News veröffentlichen bestätigen</t>
+  </si>
+  <si>
+    <t>Klick auf "News hinzufügen" und alle Felder inklusive einem Bild größer als 5 MB) ausfüllen und mit News veröffentlichen bestätigen</t>
+  </si>
+  <si>
+    <t>es kommt eine Fehlermeldung die (mehrsprachig) anzeigt, dass das Bild zu groß ist</t>
+  </si>
+  <si>
+    <t>es kommt eine Fehlermeldung die (mehrsprachig) anzeigt, welcher Text zu lang ist</t>
+  </si>
+  <si>
+    <t>es kommt eine Fehlermeldung die (mehrsprachig) anzeigt, welches Feld nicht ausgefüllt wurde</t>
   </si>
 </sst>
 </file>
@@ -465,8 +531,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A9:F400" totalsRowShown="0" headerRowDxfId="6">
-  <autoFilter ref="A9:F400"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A9:F402" totalsRowShown="0" headerRowDxfId="6">
+  <autoFilter ref="A9:F402"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Testfall #" dataDxfId="5"/>
     <tableColumn id="2" name="Testtyp" dataDxfId="4"/>
@@ -742,17 +808,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G400"/>
+  <dimension ref="A1:G402"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="15.7109375" style="1" customWidth="1"/>
-    <col min="3" max="5" width="30.7109375" style="8" customWidth="1"/>
-    <col min="6" max="6" width="35" style="8" customWidth="1"/>
+    <col min="3" max="4" width="30.7109375" style="8" customWidth="1"/>
+    <col min="5" max="6" width="35.7109375" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1124,26 +1190,145 @@
         <v>67</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="6"/>
-    </row>
-    <row r="26" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
-    </row>
-    <row r="27" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
-    </row>
-    <row r="28" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
-    </row>
-    <row r="29" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="6"/>
-    </row>
-    <row r="30" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="6"/>
-    </row>
-    <row r="31" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="6"/>
+    <row r="25" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A25" s="6">
+        <v>16</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A26" s="6">
+        <v>17</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="6">
+        <v>18</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="6">
+        <v>19</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A29" s="6">
+        <v>20</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A30" s="6">
+        <v>21</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="6">
+        <v>22</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="32" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6"/>
@@ -2251,6 +2436,12 @@
     </row>
     <row r="400" spans="1:1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A400" s="6"/>
+    </row>
+    <row r="401" spans="1:1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A401" s="6"/>
+    </row>
+    <row r="402" spans="1:1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A402" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>